<commit_message>
Add COI to master list
</commit_message>
<xml_diff>
--- a/LOI/COI/COI-all.xlsx
+++ b/LOI/COI/COI-all.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25915"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="0" windowWidth="25600" windowHeight="27040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="421">
   <si>
     <t xml:space="preserve"> UCSD</t>
   </si>
@@ -1168,6 +1168,123 @@
   </si>
   <si>
     <t>IBM</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>U. of Alabama at Birmingham</t>
+  </si>
+  <si>
+    <t>Barrett</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Brandt</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Carns</t>
+  </si>
+  <si>
+    <t>DeBardeleben</t>
+  </si>
+  <si>
+    <t>Fabian</t>
+  </si>
+  <si>
+    <t>Ferreira</t>
+  </si>
+  <si>
+    <t>Gemmill</t>
+  </si>
+  <si>
+    <t>Clemson U.</t>
+  </si>
+  <si>
+    <t>Gentile</t>
+  </si>
+  <si>
+    <t>Harms</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Hemmert</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Kimpe</t>
+  </si>
+  <si>
+    <t>Kroeger</t>
+  </si>
+  <si>
+    <t>Laros III</t>
+  </si>
+  <si>
+    <t>Leung</t>
+  </si>
+  <si>
+    <t>Levenhagen</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Pedretti</t>
+  </si>
+  <si>
+    <t>D. R.</t>
+  </si>
+  <si>
+    <t>Resnick</t>
+  </si>
+  <si>
+    <t>Ricci</t>
+  </si>
+  <si>
+    <t>U. of Utah</t>
+  </si>
+  <si>
+    <t>Rodrigues</t>
+  </si>
+  <si>
+    <t>Skjellum</t>
+  </si>
+  <si>
+    <t>Auburn U.</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Data Direct Networks</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Tucker</t>
+  </si>
+  <si>
+    <t>Van Dyke</t>
+  </si>
+  <si>
+    <t>Vaughan</t>
+  </si>
+  <si>
+    <t>Micron Technologies</t>
   </si>
 </sst>
 </file>
@@ -1253,8 +1370,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1277,9 +1398,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1582,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K307"/>
+  <dimension ref="A1:K351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D89" sqref="A89:XFD89"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H278" sqref="H278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5063,6 +5188,490 @@
         <v>351</v>
       </c>
     </row>
+    <row r="308" spans="1:3" ht="15">
+      <c r="A308" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B308" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C308" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" ht="15">
+      <c r="A309" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="B309" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C309" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" ht="15">
+      <c r="A310" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B310" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C310" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" ht="15">
+      <c r="A311" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B311" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C311" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" ht="15">
+      <c r="A312" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B312" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C312" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" ht="15">
+      <c r="A313" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B313" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C313" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3">
+      <c r="A314" t="s">
+        <v>388</v>
+      </c>
+      <c r="B314" t="s">
+        <v>36</v>
+      </c>
+      <c r="C314" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
+      <c r="A315" t="s">
+        <v>224</v>
+      </c>
+      <c r="B315" t="s">
+        <v>166</v>
+      </c>
+      <c r="C315" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3">
+      <c r="A316" t="s">
+        <v>389</v>
+      </c>
+      <c r="B316" t="s">
+        <v>103</v>
+      </c>
+      <c r="C316" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
+      <c r="A317" t="s">
+        <v>390</v>
+      </c>
+      <c r="B317" t="s">
+        <v>103</v>
+      </c>
+      <c r="C317" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
+      <c r="A318" t="s">
+        <v>391</v>
+      </c>
+      <c r="B318" t="s">
+        <v>21</v>
+      </c>
+      <c r="C318" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
+      <c r="A319" t="s">
+        <v>392</v>
+      </c>
+      <c r="B319" t="s">
+        <v>20</v>
+      </c>
+      <c r="C319" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" t="s">
+        <v>394</v>
+      </c>
+      <c r="B320" t="s">
+        <v>24</v>
+      </c>
+      <c r="C320" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
+      <c r="A321" t="s">
+        <v>395</v>
+      </c>
+      <c r="B321" t="s">
+        <v>21</v>
+      </c>
+      <c r="C321" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
+      <c r="A322" t="s">
+        <v>396</v>
+      </c>
+      <c r="B322" t="s">
+        <v>20</v>
+      </c>
+      <c r="C322" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
+      <c r="A323" t="s">
+        <v>397</v>
+      </c>
+      <c r="B323" t="s">
+        <v>28</v>
+      </c>
+      <c r="C323" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3">
+      <c r="A324" t="s">
+        <v>398</v>
+      </c>
+      <c r="B324" t="s">
+        <v>28</v>
+      </c>
+      <c r="C324" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
+      <c r="A325" t="s">
+        <v>399</v>
+      </c>
+      <c r="B325" t="s">
+        <v>87</v>
+      </c>
+      <c r="C325" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3">
+      <c r="A326" t="s">
+        <v>223</v>
+      </c>
+      <c r="B326" t="s">
+        <v>31</v>
+      </c>
+      <c r="C326" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3">
+      <c r="A327" t="s">
+        <v>400</v>
+      </c>
+      <c r="B327" t="s">
+        <v>101</v>
+      </c>
+      <c r="C327" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3">
+      <c r="A328" t="s">
+        <v>401</v>
+      </c>
+      <c r="B328" t="s">
+        <v>20</v>
+      </c>
+      <c r="C328" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3">
+      <c r="A329" t="s">
+        <v>402</v>
+      </c>
+      <c r="B329" t="s">
+        <v>37</v>
+      </c>
+      <c r="C329" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3">
+      <c r="A330" t="s">
+        <v>403</v>
+      </c>
+      <c r="B330" t="s">
+        <v>22</v>
+      </c>
+      <c r="C330" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3">
+      <c r="A331" t="s">
+        <v>53</v>
+      </c>
+      <c r="B331" t="s">
+        <v>166</v>
+      </c>
+      <c r="C331" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3">
+      <c r="A332" t="s">
+        <v>404</v>
+      </c>
+      <c r="B332" t="s">
+        <v>87</v>
+      </c>
+      <c r="C332" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3">
+      <c r="A333" t="s">
+        <v>370</v>
+      </c>
+      <c r="B333" t="s">
+        <v>26</v>
+      </c>
+      <c r="C333" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334" t="s">
+        <v>405</v>
+      </c>
+      <c r="B334" t="s">
+        <v>29</v>
+      </c>
+      <c r="C334" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3">
+      <c r="A335" t="s">
+        <v>80</v>
+      </c>
+      <c r="B335" t="s">
+        <v>21</v>
+      </c>
+      <c r="C335" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3">
+      <c r="A336" t="s">
+        <v>54</v>
+      </c>
+      <c r="B336" t="s">
+        <v>31</v>
+      </c>
+      <c r="C336" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3">
+      <c r="A337" t="s">
+        <v>406</v>
+      </c>
+      <c r="B337" t="s">
+        <v>21</v>
+      </c>
+      <c r="C337" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338" t="s">
+        <v>408</v>
+      </c>
+      <c r="B338" t="s">
+        <v>407</v>
+      </c>
+      <c r="C338" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="A339" t="s">
+        <v>409</v>
+      </c>
+      <c r="B339" t="s">
+        <v>31</v>
+      </c>
+      <c r="C339" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3">
+      <c r="A340" t="s">
+        <v>411</v>
+      </c>
+      <c r="B340" t="s">
+        <v>24</v>
+      </c>
+      <c r="C340" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3">
+      <c r="A341" t="s">
+        <v>280</v>
+      </c>
+      <c r="B341" t="s">
+        <v>31</v>
+      </c>
+      <c r="C341" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3">
+      <c r="A342" t="s">
+        <v>82</v>
+      </c>
+      <c r="B342" t="s">
+        <v>38</v>
+      </c>
+      <c r="C342" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3">
+      <c r="A343" t="s">
+        <v>412</v>
+      </c>
+      <c r="B343" t="s">
+        <v>24</v>
+      </c>
+      <c r="C343" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3">
+      <c r="A344" t="s">
+        <v>414</v>
+      </c>
+      <c r="B344" t="s">
+        <v>23</v>
+      </c>
+      <c r="C344" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3">
+      <c r="A345" t="s">
+        <v>414</v>
+      </c>
+      <c r="B345" t="s">
+        <v>33</v>
+      </c>
+      <c r="C345" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3">
+      <c r="A346" t="s">
+        <v>416</v>
+      </c>
+      <c r="B346" t="s">
+        <v>87</v>
+      </c>
+      <c r="C346" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3">
+      <c r="A347" t="s">
+        <v>417</v>
+      </c>
+      <c r="B347" t="s">
+        <v>101</v>
+      </c>
+      <c r="C347" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3">
+      <c r="A348" t="s">
+        <v>418</v>
+      </c>
+      <c r="B348" t="s">
+        <v>20</v>
+      </c>
+      <c r="C348" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3">
+      <c r="A349" t="s">
+        <v>419</v>
+      </c>
+      <c r="B349" t="s">
+        <v>26</v>
+      </c>
+      <c r="C349" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3">
+      <c r="A350" t="s">
+        <v>221</v>
+      </c>
+      <c r="B350" t="s">
+        <v>154</v>
+      </c>
+      <c r="C350" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3">
+      <c r="A351" t="s">
+        <v>289</v>
+      </c>
+      <c r="B351" t="s">
+        <v>21</v>
+      </c>
+      <c r="C351" t="s">
+        <v>420</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C63">
     <sortCondition ref="A2:A63"/>

</xml_diff>

<commit_message>
added a couple of forgotten COIs
</commit_message>
<xml_diff>
--- a/LOI/COI/COI-all.xlsx
+++ b/LOI/COI/COI-all.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="424">
   <si>
     <t xml:space="preserve"> UCSD</t>
   </si>
@@ -1285,6 +1285,15 @@
   </si>
   <si>
     <t>Micron Technologies</t>
+  </si>
+  <si>
+    <t>Lang</t>
+  </si>
+  <si>
+    <t>Lange</t>
+  </si>
+  <si>
+    <t>Univeristy of Pittsburgh</t>
   </si>
 </sst>
 </file>
@@ -1707,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K351"/>
+  <dimension ref="A1:K353"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H278" sqref="H278"/>
+    <sheetView tabSelected="1" topLeftCell="A330" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A354" sqref="A354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5672,6 +5681,28 @@
         <v>420</v>
       </c>
     </row>
+    <row r="352" spans="1:3">
+      <c r="A352" t="s">
+        <v>421</v>
+      </c>
+      <c r="B352" t="s">
+        <v>22</v>
+      </c>
+      <c r="C352" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3">
+      <c r="A353" t="s">
+        <v>422</v>
+      </c>
+      <c r="B353" t="s">
+        <v>20</v>
+      </c>
+      <c r="C353" t="s">
+        <v>423</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C63">
     <sortCondition ref="A2:A63"/>

</xml_diff>

<commit_message>
modified:   COI-all.xlsx 	modified:   coi_maltzahn.txt
</commit_message>
<xml_diff>
--- a/LOI/COI/COI-all.xlsx
+++ b/LOI/COI/COI-all.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1740" yWindow="-21580" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Carlos" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="coi_maltzahn" localSheetId="1">Carlos!$A$1:$D$55</definedName>
+    <definedName name="coi_maltzahn" localSheetId="0">Sheet1!$A$354:$D$408</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">Sheet1!$A$2</definedName>
   </definedNames>
   <calcPr calcId="122211" concurrentCalc="0"/>
@@ -21,8 +24,33 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="coi_maltzahn.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:carlosmalt:git:ssio-proposal:LOI:COI:coi_maltzahn.txt" tab="0" semicolon="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="coi_maltzahn.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:carlosmalt:git:ssio-proposal:LOI:COI:coi_maltzahn.txt" tab="0" semicolon="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="505">
   <si>
     <t xml:space="preserve"> UCSD</t>
   </si>
@@ -1294,6 +1322,249 @@
   </si>
   <si>
     <t>Univeristy of Pittsburgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Achlioptas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> co-author</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ames</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arpaci-Dusseau</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EMC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bhagwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yahoo!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brandt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Buck</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Context Relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carns</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carothers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rensselaer Polytechnic Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cope</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DDN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Curry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dayal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gibson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gokhale</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grandison</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Proficiency Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grider</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grunwald</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> advisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> He</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hjelm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> collaborator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ioannidou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TidalScale</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ionkov</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jhala</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kato</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nagoya University</t>
+  </si>
+  <si>
+    <t>Q.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Koziol</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HDF Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kroeger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Levin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Google</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lofstead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> affiliation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manzanares</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HGST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mateas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> McCormick</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Miller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mohror</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moody</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nassi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Obraczka</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oldfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Polyzotis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pye</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cloud Helix</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ross</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shewmaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shipman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Skourtis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VMWare</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Illinois Institute of Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Torres</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Linden Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Weil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Red Hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Whitehead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Widener</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wolpert</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Woodring</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UCSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ANL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SNL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LANL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UW Madison</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CMU</t>
   </si>
 </sst>
 </file>
@@ -1379,8 +1650,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1407,13 +1682,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1427,6 +1706,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="coi_maltzahn" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="coi_maltzahn" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1716,10 +2003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K353"/>
+  <dimension ref="A1:K408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A354" sqref="A354"/>
+    <sheetView tabSelected="1" topLeftCell="A383" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A354" sqref="A354:D408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5692,7 +5979,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="353" spans="1:3">
+    <row r="353" spans="1:4">
       <c r="A353" t="s">
         <v>422</v>
       </c>
@@ -5701,6 +5988,776 @@
       </c>
       <c r="C353" t="s">
         <v>423</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4">
+      <c r="A354" t="s">
+        <v>424</v>
+      </c>
+      <c r="B354" t="s">
+        <v>87</v>
+      </c>
+      <c r="C354" t="s">
+        <v>499</v>
+      </c>
+      <c r="D354" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4">
+      <c r="A355" t="s">
+        <v>426</v>
+      </c>
+      <c r="B355" t="s">
+        <v>28</v>
+      </c>
+      <c r="C355" t="s">
+        <v>11</v>
+      </c>
+      <c r="D355" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4">
+      <c r="A356" t="s">
+        <v>427</v>
+      </c>
+      <c r="B356" t="s">
+        <v>24</v>
+      </c>
+      <c r="C356" t="s">
+        <v>503</v>
+      </c>
+      <c r="D356" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4">
+      <c r="A357" t="s">
+        <v>427</v>
+      </c>
+      <c r="B357" t="s">
+        <v>31</v>
+      </c>
+      <c r="C357" t="s">
+        <v>503</v>
+      </c>
+      <c r="D357" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4">
+      <c r="A358" t="s">
+        <v>428</v>
+      </c>
+      <c r="B358" t="s">
+        <v>20</v>
+      </c>
+      <c r="C358" t="s">
+        <v>429</v>
+      </c>
+      <c r="D358" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4">
+      <c r="A359" t="s">
+        <v>430</v>
+      </c>
+      <c r="B359" t="s">
+        <v>37</v>
+      </c>
+      <c r="C359" t="s">
+        <v>431</v>
+      </c>
+      <c r="D359" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4">
+      <c r="A360" t="s">
+        <v>432</v>
+      </c>
+      <c r="B360" t="s">
+        <v>28</v>
+      </c>
+      <c r="C360" t="s">
+        <v>499</v>
+      </c>
+      <c r="D360" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4">
+      <c r="A361" t="s">
+        <v>433</v>
+      </c>
+      <c r="B361" t="s">
+        <v>20</v>
+      </c>
+      <c r="C361" t="s">
+        <v>434</v>
+      </c>
+      <c r="D361" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4">
+      <c r="A362" t="s">
+        <v>435</v>
+      </c>
+      <c r="B362" t="s">
+        <v>36</v>
+      </c>
+      <c r="C362" t="s">
+        <v>500</v>
+      </c>
+      <c r="D362" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4">
+      <c r="A363" t="s">
+        <v>436</v>
+      </c>
+      <c r="B363" t="s">
+        <v>26</v>
+      </c>
+      <c r="C363" t="s">
+        <v>437</v>
+      </c>
+      <c r="D363" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4">
+      <c r="A364" t="s">
+        <v>438</v>
+      </c>
+      <c r="B364" t="s">
+        <v>20</v>
+      </c>
+      <c r="C364" t="s">
+        <v>439</v>
+      </c>
+      <c r="D364" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4">
+      <c r="A365" t="s">
+        <v>440</v>
+      </c>
+      <c r="B365" t="s">
+        <v>22</v>
+      </c>
+      <c r="C365" t="s">
+        <v>501</v>
+      </c>
+      <c r="D365" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4">
+      <c r="A366" t="s">
+        <v>441</v>
+      </c>
+      <c r="B366" t="s">
+        <v>20</v>
+      </c>
+      <c r="C366" t="s">
+        <v>12</v>
+      </c>
+      <c r="D366" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4">
+      <c r="A367" t="s">
+        <v>442</v>
+      </c>
+      <c r="B367" t="s">
+        <v>166</v>
+      </c>
+      <c r="C367" t="s">
+        <v>504</v>
+      </c>
+      <c r="D367" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4">
+      <c r="A368" t="s">
+        <v>443</v>
+      </c>
+      <c r="B368" t="s">
+        <v>22</v>
+      </c>
+      <c r="C368" t="s">
+        <v>11</v>
+      </c>
+      <c r="D368" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4">
+      <c r="A369" t="s">
+        <v>444</v>
+      </c>
+      <c r="B369" t="s">
+        <v>101</v>
+      </c>
+      <c r="C369" t="s">
+        <v>445</v>
+      </c>
+      <c r="D369" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4">
+      <c r="A370" t="s">
+        <v>446</v>
+      </c>
+      <c r="B370" t="s">
+        <v>166</v>
+      </c>
+      <c r="C370" t="s">
+        <v>502</v>
+      </c>
+      <c r="D370" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4">
+      <c r="A371" t="s">
+        <v>447</v>
+      </c>
+      <c r="B371" t="s">
+        <v>87</v>
+      </c>
+      <c r="C371" t="s">
+        <v>499</v>
+      </c>
+      <c r="D371" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4">
+      <c r="A372" t="s">
+        <v>449</v>
+      </c>
+      <c r="B372" t="s">
+        <v>20</v>
+      </c>
+      <c r="C372" t="s">
+        <v>503</v>
+      </c>
+      <c r="D372" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4">
+      <c r="A373" t="s">
+        <v>450</v>
+      </c>
+      <c r="B373" t="s">
+        <v>103</v>
+      </c>
+      <c r="C373" t="s">
+        <v>502</v>
+      </c>
+      <c r="D373" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4">
+      <c r="A374" t="s">
+        <v>452</v>
+      </c>
+      <c r="B374" t="s">
+        <v>21</v>
+      </c>
+      <c r="C374" t="s">
+        <v>453</v>
+      </c>
+      <c r="D374" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4">
+      <c r="A375" t="s">
+        <v>454</v>
+      </c>
+      <c r="B375" t="s">
+        <v>154</v>
+      </c>
+      <c r="C375" t="s">
+        <v>502</v>
+      </c>
+      <c r="D375" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4">
+      <c r="A376" t="s">
+        <v>455</v>
+      </c>
+      <c r="B376" t="s">
+        <v>24</v>
+      </c>
+      <c r="C376" t="s">
+        <v>499</v>
+      </c>
+      <c r="D376" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4">
+      <c r="A377" t="s">
+        <v>456</v>
+      </c>
+      <c r="B377" t="s">
+        <v>28</v>
+      </c>
+      <c r="C377" t="s">
+        <v>457</v>
+      </c>
+      <c r="D377" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4">
+      <c r="A378" t="s">
+        <v>459</v>
+      </c>
+      <c r="B378" t="s">
+        <v>458</v>
+      </c>
+      <c r="C378" t="s">
+        <v>460</v>
+      </c>
+      <c r="D378" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4">
+      <c r="A379" t="s">
+        <v>461</v>
+      </c>
+      <c r="B379" t="s">
+        <v>101</v>
+      </c>
+      <c r="C379" t="s">
+        <v>501</v>
+      </c>
+      <c r="D379" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4">
+      <c r="A380" t="s">
+        <v>462</v>
+      </c>
+      <c r="B380" t="s">
+        <v>22</v>
+      </c>
+      <c r="C380" t="s">
+        <v>502</v>
+      </c>
+      <c r="D380" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4">
+      <c r="A381" t="s">
+        <v>463</v>
+      </c>
+      <c r="B381" t="s">
+        <v>166</v>
+      </c>
+      <c r="C381" t="s">
+        <v>464</v>
+      </c>
+      <c r="D381" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4">
+      <c r="A382" t="s">
+        <v>465</v>
+      </c>
+      <c r="B382" t="s">
+        <v>103</v>
+      </c>
+      <c r="C382" t="s">
+        <v>500</v>
+      </c>
+      <c r="D382" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4">
+      <c r="A383" t="s">
+        <v>466</v>
+      </c>
+      <c r="B383" t="s">
+        <v>20</v>
+      </c>
+      <c r="C383" t="s">
+        <v>501</v>
+      </c>
+      <c r="D383" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4">
+      <c r="A384" t="s">
+        <v>467</v>
+      </c>
+      <c r="B384" t="s">
+        <v>87</v>
+      </c>
+      <c r="C384" t="s">
+        <v>499</v>
+      </c>
+      <c r="D384" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4">
+      <c r="A385" t="s">
+        <v>469</v>
+      </c>
+      <c r="B385" t="s">
+        <v>24</v>
+      </c>
+      <c r="C385" t="s">
+        <v>470</v>
+      </c>
+      <c r="D385" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4">
+      <c r="A386" t="s">
+        <v>471</v>
+      </c>
+      <c r="B386" t="s">
+        <v>22</v>
+      </c>
+      <c r="C386" t="s">
+        <v>499</v>
+      </c>
+      <c r="D386" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4">
+      <c r="A387" t="s">
+        <v>472</v>
+      </c>
+      <c r="B387" t="s">
+        <v>36</v>
+      </c>
+      <c r="C387" t="s">
+        <v>502</v>
+      </c>
+      <c r="D387" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4">
+      <c r="A388" t="s">
+        <v>473</v>
+      </c>
+      <c r="B388" t="s">
+        <v>29</v>
+      </c>
+      <c r="C388" t="s">
+        <v>499</v>
+      </c>
+      <c r="D388" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4">
+      <c r="A389" t="s">
+        <v>474</v>
+      </c>
+      <c r="B389" t="s">
+        <v>21</v>
+      </c>
+      <c r="C389" t="s">
+        <v>11</v>
+      </c>
+      <c r="D389" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4">
+      <c r="A390" t="s">
+        <v>475</v>
+      </c>
+      <c r="B390" t="s">
+        <v>24</v>
+      </c>
+      <c r="C390" t="s">
+        <v>11</v>
+      </c>
+      <c r="D390" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4">
+      <c r="A391" t="s">
+        <v>476</v>
+      </c>
+      <c r="B391" t="s">
+        <v>35</v>
+      </c>
+      <c r="C391" t="s">
+        <v>453</v>
+      </c>
+      <c r="D391" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4">
+      <c r="A392" t="s">
+        <v>477</v>
+      </c>
+      <c r="B392" t="s">
+        <v>21</v>
+      </c>
+      <c r="C392" t="s">
+        <v>499</v>
+      </c>
+      <c r="D392" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4">
+      <c r="A393" t="s">
+        <v>478</v>
+      </c>
+      <c r="B393" t="s">
+        <v>31</v>
+      </c>
+      <c r="C393" t="s">
+        <v>501</v>
+      </c>
+      <c r="D393" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4">
+      <c r="A394" t="s">
+        <v>479</v>
+      </c>
+      <c r="B394" t="s">
+        <v>103</v>
+      </c>
+      <c r="C394" t="s">
+        <v>464</v>
+      </c>
+      <c r="D394" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4">
+      <c r="A395" t="s">
+        <v>480</v>
+      </c>
+      <c r="B395" t="s">
+        <v>35</v>
+      </c>
+      <c r="C395" t="s">
+        <v>481</v>
+      </c>
+      <c r="D395" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4">
+      <c r="A396" t="s">
+        <v>482</v>
+      </c>
+      <c r="B396" t="s">
+        <v>31</v>
+      </c>
+      <c r="C396" t="s">
+        <v>500</v>
+      </c>
+      <c r="D396" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4">
+      <c r="A397" t="s">
+        <v>483</v>
+      </c>
+      <c r="B397" t="s">
+        <v>24</v>
+      </c>
+      <c r="C397" t="s">
+        <v>502</v>
+      </c>
+      <c r="D397" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4">
+      <c r="A398" t="s">
+        <v>484</v>
+      </c>
+      <c r="B398" t="s">
+        <v>166</v>
+      </c>
+      <c r="C398" t="s">
+        <v>502</v>
+      </c>
+      <c r="D398" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4">
+      <c r="A399" t="s">
+        <v>485</v>
+      </c>
+      <c r="B399" t="s">
+        <v>87</v>
+      </c>
+      <c r="C399" t="s">
+        <v>486</v>
+      </c>
+      <c r="D399" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4">
+      <c r="A400" t="s">
+        <v>487</v>
+      </c>
+      <c r="B400" t="s">
+        <v>134</v>
+      </c>
+      <c r="C400" t="s">
+        <v>488</v>
+      </c>
+      <c r="D400" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4">
+      <c r="A401" t="s">
+        <v>489</v>
+      </c>
+      <c r="B401" t="s">
+        <v>23</v>
+      </c>
+      <c r="C401" t="s">
+        <v>499</v>
+      </c>
+      <c r="D401" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4">
+      <c r="A402" t="s">
+        <v>490</v>
+      </c>
+      <c r="B402" t="s">
+        <v>24</v>
+      </c>
+      <c r="C402" t="s">
+        <v>491</v>
+      </c>
+      <c r="D402" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4">
+      <c r="A403" t="s">
+        <v>492</v>
+      </c>
+      <c r="B403" t="s">
+        <v>154</v>
+      </c>
+      <c r="C403" t="s">
+        <v>501</v>
+      </c>
+      <c r="D403" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4">
+      <c r="A404" t="s">
+        <v>493</v>
+      </c>
+      <c r="B404" t="s">
+        <v>28</v>
+      </c>
+      <c r="C404" t="s">
+        <v>494</v>
+      </c>
+      <c r="D404" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4">
+      <c r="A405" t="s">
+        <v>495</v>
+      </c>
+      <c r="B405" t="s">
+        <v>20</v>
+      </c>
+      <c r="C405" t="s">
+        <v>499</v>
+      </c>
+      <c r="D405" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4">
+      <c r="A406" t="s">
+        <v>496</v>
+      </c>
+      <c r="B406" t="s">
+        <v>36</v>
+      </c>
+      <c r="C406" t="s">
+        <v>501</v>
+      </c>
+      <c r="D406" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4">
+      <c r="A407" t="s">
+        <v>497</v>
+      </c>
+      <c r="B407" t="s">
+        <v>87</v>
+      </c>
+      <c r="C407" t="s">
+        <v>502</v>
+      </c>
+      <c r="D407" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4">
+      <c r="A408" t="s">
+        <v>498</v>
+      </c>
+      <c r="B408" t="s">
+        <v>20</v>
+      </c>
+      <c r="C408" t="s">
+        <v>502</v>
+      </c>
+      <c r="D408" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -5715,4 +6772,800 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>503</v>
+      </c>
+      <c r="D3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>503</v>
+      </c>
+      <c r="D4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>432</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>499</v>
+      </c>
+      <c r="D7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>433</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>435</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>500</v>
+      </c>
+      <c r="D9" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>437</v>
+      </c>
+      <c r="D10" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>439</v>
+      </c>
+      <c r="D11" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>501</v>
+      </c>
+      <c r="D12" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>441</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>442</v>
+      </c>
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" t="s">
+        <v>504</v>
+      </c>
+      <c r="D14" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>444</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>445</v>
+      </c>
+      <c r="D16" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>446</v>
+      </c>
+      <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" t="s">
+        <v>502</v>
+      </c>
+      <c r="D17" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>447</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>499</v>
+      </c>
+      <c r="D18" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>449</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>503</v>
+      </c>
+      <c r="D19" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>450</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>502</v>
+      </c>
+      <c r="D20" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>452</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>453</v>
+      </c>
+      <c r="D21" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>454</v>
+      </c>
+      <c r="B22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" t="s">
+        <v>502</v>
+      </c>
+      <c r="D22" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>455</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>499</v>
+      </c>
+      <c r="D23" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>456</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>457</v>
+      </c>
+      <c r="D24" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>459</v>
+      </c>
+      <c r="B25" t="s">
+        <v>458</v>
+      </c>
+      <c r="C25" t="s">
+        <v>460</v>
+      </c>
+      <c r="D25" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>461</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>501</v>
+      </c>
+      <c r="D26" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>462</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>502</v>
+      </c>
+      <c r="D27" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>463</v>
+      </c>
+      <c r="B28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" t="s">
+        <v>464</v>
+      </c>
+      <c r="D28" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>465</v>
+      </c>
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s">
+        <v>500</v>
+      </c>
+      <c r="D29" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>466</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>501</v>
+      </c>
+      <c r="D30" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>467</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>499</v>
+      </c>
+      <c r="D31" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>469</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>470</v>
+      </c>
+      <c r="D32" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>471</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>499</v>
+      </c>
+      <c r="D33" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>472</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>502</v>
+      </c>
+      <c r="D34" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>473</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>499</v>
+      </c>
+      <c r="D35" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>474</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>475</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>476</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>453</v>
+      </c>
+      <c r="D38" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>477</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" t="s">
+        <v>499</v>
+      </c>
+      <c r="D39" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>478</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>501</v>
+      </c>
+      <c r="D40" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>479</v>
+      </c>
+      <c r="B41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" t="s">
+        <v>464</v>
+      </c>
+      <c r="D41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>480</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>481</v>
+      </c>
+      <c r="D42" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>482</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" t="s">
+        <v>500</v>
+      </c>
+      <c r="D43" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>483</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>502</v>
+      </c>
+      <c r="D44" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>484</v>
+      </c>
+      <c r="B45" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" t="s">
+        <v>502</v>
+      </c>
+      <c r="D45" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>485</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>486</v>
+      </c>
+      <c r="D46" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>487</v>
+      </c>
+      <c r="B47" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" t="s">
+        <v>488</v>
+      </c>
+      <c r="D47" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>489</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" t="s">
+        <v>499</v>
+      </c>
+      <c r="D48" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>490</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" t="s">
+        <v>491</v>
+      </c>
+      <c r="D49" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>492</v>
+      </c>
+      <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>501</v>
+      </c>
+      <c r="D50" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>493</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>494</v>
+      </c>
+      <c r="D51" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>495</v>
+      </c>
+      <c r="B52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" t="s">
+        <v>499</v>
+      </c>
+      <c r="D52" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>496</v>
+      </c>
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" t="s">
+        <v>501</v>
+      </c>
+      <c r="D53" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>497</v>
+      </c>
+      <c r="B54" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" t="s">
+        <v>502</v>
+      </c>
+      <c r="D54" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>498</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>502</v>
+      </c>
+      <c r="D55" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added conflict information to my entries.
</commit_message>
<xml_diff>
--- a/LOI/COI/COI-all.xlsx
+++ b/LOI/COI/COI-all.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25915"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="-21580" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="coi_maltzahn.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:carlosmalt:git:ssio-proposal:LOI:COI:coi_maltzahn.txt" tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:carlosmalt:git:ssio-proposal:LOI:COI:coi_maltzahn.txt" tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -37,7 +37,7 @@
     </textPr>
   </connection>
   <connection id="2" name="coi_maltzahn.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:carlosmalt:git:ssio-proposal:LOI:COI:coi_maltzahn.txt" tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:carlosmalt:git:ssio-proposal:LOI:COI:coi_maltzahn.txt" tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="507">
   <si>
     <t xml:space="preserve"> UCSD</t>
   </si>
@@ -1565,6 +1565,12 @@
   </si>
   <si>
     <t xml:space="preserve"> CMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> co-author, collaborator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> co-author, collaborator, advisor</t>
   </si>
 </sst>
 </file>
@@ -2005,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A383" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A354" sqref="A354:D408"/>
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F344" sqref="F344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5451,7 +5457,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="305" spans="1:3" ht="15">
+    <row r="305" spans="1:4" ht="15">
       <c r="A305" s="6" t="s">
         <v>347</v>
       </c>
@@ -5462,7 +5468,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="15">
+    <row r="306" spans="1:4" ht="15">
       <c r="A306" s="6" t="s">
         <v>349</v>
       </c>
@@ -5473,7 +5479,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="307" spans="1:3" ht="15">
+    <row r="307" spans="1:4" ht="15">
       <c r="A307" s="6" t="s">
         <v>350</v>
       </c>
@@ -5484,7 +5490,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="308" spans="1:3" ht="15">
+    <row r="308" spans="1:4" ht="15">
       <c r="A308" s="6" t="s">
         <v>352</v>
       </c>
@@ -5494,8 +5500,11 @@
       <c r="C308" s="6" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" ht="15">
+      <c r="D308" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" ht="15">
       <c r="A309" s="6" t="s">
         <v>382</v>
       </c>
@@ -5505,8 +5514,11 @@
       <c r="C309" s="6" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" ht="15">
+      <c r="D309" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" ht="15">
       <c r="A310" s="6" t="s">
         <v>384</v>
       </c>
@@ -5516,8 +5528,11 @@
       <c r="C310" s="6" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" ht="15">
+      <c r="D310" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" ht="15">
       <c r="A311" s="6" t="s">
         <v>384</v>
       </c>
@@ -5527,8 +5542,11 @@
       <c r="C311" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" ht="15">
+      <c r="D311" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" ht="15">
       <c r="A312" s="6" t="s">
         <v>386</v>
       </c>
@@ -5538,8 +5556,11 @@
       <c r="C312" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" ht="15">
+      <c r="D312" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" ht="15">
       <c r="A313" s="6" t="s">
         <v>65</v>
       </c>
@@ -5549,8 +5570,11 @@
       <c r="C313" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="314" spans="1:3">
+      <c r="D313" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4">
       <c r="A314" t="s">
         <v>388</v>
       </c>
@@ -5560,8 +5584,11 @@
       <c r="C314" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="315" spans="1:3">
+      <c r="D314" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4">
       <c r="A315" t="s">
         <v>224</v>
       </c>
@@ -5571,8 +5598,11 @@
       <c r="C315" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="316" spans="1:3">
+      <c r="D315" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4">
       <c r="A316" t="s">
         <v>389</v>
       </c>
@@ -5582,8 +5612,11 @@
       <c r="C316" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="317" spans="1:3">
+      <c r="D316" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4">
       <c r="A317" t="s">
         <v>390</v>
       </c>
@@ -5593,8 +5626,11 @@
       <c r="C317" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="318" spans="1:3">
+      <c r="D317" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4">
       <c r="A318" t="s">
         <v>391</v>
       </c>
@@ -5604,8 +5640,11 @@
       <c r="C318" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="319" spans="1:3">
+      <c r="D318" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4">
       <c r="A319" t="s">
         <v>392</v>
       </c>
@@ -5615,8 +5654,11 @@
       <c r="C319" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="320" spans="1:3">
+      <c r="D319" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4">
       <c r="A320" t="s">
         <v>394</v>
       </c>
@@ -5626,8 +5668,11 @@
       <c r="C320" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="321" spans="1:3">
+      <c r="D320" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4">
       <c r="A321" t="s">
         <v>395</v>
       </c>
@@ -5637,8 +5682,11 @@
       <c r="C321" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="322" spans="1:3">
+      <c r="D321" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4">
       <c r="A322" t="s">
         <v>396</v>
       </c>
@@ -5648,8 +5696,11 @@
       <c r="C322" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="323" spans="1:3">
+      <c r="D322" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4">
       <c r="A323" t="s">
         <v>397</v>
       </c>
@@ -5659,8 +5710,11 @@
       <c r="C323" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="324" spans="1:3">
+      <c r="D323" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4">
       <c r="A324" t="s">
         <v>398</v>
       </c>
@@ -5670,8 +5724,11 @@
       <c r="C324" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="325" spans="1:3">
+      <c r="D324" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4">
       <c r="A325" t="s">
         <v>399</v>
       </c>
@@ -5681,8 +5738,11 @@
       <c r="C325" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="326" spans="1:3">
+      <c r="D325" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4">
       <c r="A326" t="s">
         <v>223</v>
       </c>
@@ -5692,8 +5752,11 @@
       <c r="C326" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="327" spans="1:3">
+      <c r="D326" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4">
       <c r="A327" t="s">
         <v>400</v>
       </c>
@@ -5703,8 +5766,11 @@
       <c r="C327" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="328" spans="1:3">
+      <c r="D327" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4">
       <c r="A328" t="s">
         <v>401</v>
       </c>
@@ -5714,8 +5780,11 @@
       <c r="C328" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="329" spans="1:3">
+      <c r="D328" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4">
       <c r="A329" t="s">
         <v>402</v>
       </c>
@@ -5725,8 +5794,11 @@
       <c r="C329" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="330" spans="1:3">
+      <c r="D329" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4">
       <c r="A330" t="s">
         <v>403</v>
       </c>
@@ -5736,8 +5808,11 @@
       <c r="C330" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="331" spans="1:3">
+      <c r="D330" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4">
       <c r="A331" t="s">
         <v>53</v>
       </c>
@@ -5747,8 +5822,11 @@
       <c r="C331" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="332" spans="1:3">
+      <c r="D331" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4">
       <c r="A332" t="s">
         <v>404</v>
       </c>
@@ -5758,8 +5836,11 @@
       <c r="C332" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="333" spans="1:3">
+      <c r="D332" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4">
       <c r="A333" t="s">
         <v>370</v>
       </c>
@@ -5769,8 +5850,11 @@
       <c r="C333" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="334" spans="1:3">
+      <c r="D333" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4">
       <c r="A334" t="s">
         <v>405</v>
       </c>
@@ -5780,8 +5864,11 @@
       <c r="C334" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="335" spans="1:3">
+      <c r="D334" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4">
       <c r="A335" t="s">
         <v>80</v>
       </c>
@@ -5791,8 +5878,11 @@
       <c r="C335" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="336" spans="1:3">
+      <c r="D335" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4">
       <c r="A336" t="s">
         <v>54</v>
       </c>
@@ -5802,8 +5892,11 @@
       <c r="C336" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="337" spans="1:3">
+      <c r="D336" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4">
       <c r="A337" t="s">
         <v>406</v>
       </c>
@@ -5813,8 +5906,11 @@
       <c r="C337" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="338" spans="1:3">
+      <c r="D337" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4">
       <c r="A338" t="s">
         <v>408</v>
       </c>
@@ -5824,8 +5920,11 @@
       <c r="C338" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="339" spans="1:3">
+      <c r="D338" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4">
       <c r="A339" t="s">
         <v>409</v>
       </c>
@@ -5835,8 +5934,11 @@
       <c r="C339" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="340" spans="1:3">
+      <c r="D339" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4">
       <c r="A340" t="s">
         <v>411</v>
       </c>
@@ -5846,8 +5948,11 @@
       <c r="C340" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="341" spans="1:3">
+      <c r="D340" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4">
       <c r="A341" t="s">
         <v>280</v>
       </c>
@@ -5857,8 +5962,11 @@
       <c r="C341" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="342" spans="1:3">
+      <c r="D341" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4">
       <c r="A342" t="s">
         <v>82</v>
       </c>
@@ -5868,8 +5976,11 @@
       <c r="C342" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="343" spans="1:3">
+      <c r="D342" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4">
       <c r="A343" t="s">
         <v>412</v>
       </c>
@@ -5879,8 +5990,11 @@
       <c r="C343" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="344" spans="1:3">
+      <c r="D343" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4">
       <c r="A344" t="s">
         <v>414</v>
       </c>
@@ -5890,8 +6004,11 @@
       <c r="C344" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="345" spans="1:3">
+      <c r="D344" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4">
       <c r="A345" t="s">
         <v>414</v>
       </c>
@@ -5901,8 +6018,11 @@
       <c r="C345" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="346" spans="1:3">
+      <c r="D345" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4">
       <c r="A346" t="s">
         <v>416</v>
       </c>
@@ -5912,8 +6032,11 @@
       <c r="C346" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="347" spans="1:3">
+      <c r="D346" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4">
       <c r="A347" t="s">
         <v>417</v>
       </c>
@@ -5923,8 +6046,11 @@
       <c r="C347" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="348" spans="1:3">
+      <c r="D347" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4">
       <c r="A348" t="s">
         <v>418</v>
       </c>
@@ -5934,8 +6060,11 @@
       <c r="C348" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="349" spans="1:3">
+      <c r="D348" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4">
       <c r="A349" t="s">
         <v>419</v>
       </c>
@@ -5945,8 +6074,11 @@
       <c r="C349" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="350" spans="1:3">
+      <c r="D349" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4">
       <c r="A350" t="s">
         <v>221</v>
       </c>
@@ -5956,8 +6088,11 @@
       <c r="C350" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="351" spans="1:3">
+      <c r="D350" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4">
       <c r="A351" t="s">
         <v>289</v>
       </c>
@@ -5967,8 +6102,11 @@
       <c r="C351" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="352" spans="1:3">
+      <c r="D351" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4">
       <c r="A352" t="s">
         <v>421</v>
       </c>

</xml_diff>